<commit_message>
Final code and supplemental files
</commit_message>
<xml_diff>
--- a/SigGenesFormatted.xlsx
+++ b/SigGenesFormatted.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngsim\Documents\UCLA\BE188\Final\BE188_Final_Project-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73DE752B-901A-46DA-9D4C-A83F75350081}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84A93AB-7DC4-46E5-943C-A173AD781483}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="8Sig" sheetId="1" r:id="rId1"/>
+    <sheet name="7Sig" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="142">
   <si>
     <t>A_23_P107744</t>
   </si>
@@ -230,6 +231,222 @@
   </si>
   <si>
     <t>Transcript stable ID</t>
+  </si>
+  <si>
+    <t>A_23_P1014</t>
+  </si>
+  <si>
+    <t>A_23_P122906</t>
+  </si>
+  <si>
+    <t>A_23_P126836</t>
+  </si>
+  <si>
+    <t>A_23_P13031</t>
+  </si>
+  <si>
+    <t>A_23_P130815</t>
+  </si>
+  <si>
+    <t>A_23_P130836</t>
+  </si>
+  <si>
+    <t>A_23_P139632</t>
+  </si>
+  <si>
+    <t>A_23_P139654</t>
+  </si>
+  <si>
+    <t>A_23_P144668</t>
+  </si>
+  <si>
+    <t>A_23_P150053</t>
+  </si>
+  <si>
+    <t>A_23_P152559</t>
+  </si>
+  <si>
+    <t>A_23_P152838</t>
+  </si>
+  <si>
+    <t>A_23_P157038</t>
+  </si>
+  <si>
+    <t>A_23_P165343</t>
+  </si>
+  <si>
+    <t>A_23_P212792</t>
+  </si>
+  <si>
+    <t>A_23_P22232</t>
+  </si>
+  <si>
+    <t>A_23_P23221</t>
+  </si>
+  <si>
+    <t>A_23_P259141</t>
+  </si>
+  <si>
+    <t>A_23_P312920</t>
+  </si>
+  <si>
+    <t>A_23_P314712</t>
+  </si>
+  <si>
+    <t>A_23_P334218</t>
+  </si>
+  <si>
+    <t>A_23_P351148</t>
+  </si>
+  <si>
+    <t>A_23_P357717</t>
+  </si>
+  <si>
+    <t>A_23_P357936</t>
+  </si>
+  <si>
+    <t>A_23_P38154</t>
+  </si>
+  <si>
+    <t>A_23_P391344</t>
+  </si>
+  <si>
+    <t>A_23_P397937</t>
+  </si>
+  <si>
+    <t>A_23_P406341</t>
+  </si>
+  <si>
+    <t>A_23_P43157</t>
+  </si>
+  <si>
+    <t>A_23_P52610</t>
+  </si>
+  <si>
+    <t>A_23_P59543</t>
+  </si>
+  <si>
+    <t>A_23_P66881</t>
+  </si>
+  <si>
+    <t>A_23_P70318</t>
+  </si>
+  <si>
+    <t>A_23_P71790</t>
+  </si>
+  <si>
+    <t>A_23_P80068</t>
+  </si>
+  <si>
+    <t>A_23_P80528</t>
+  </si>
+  <si>
+    <t>A_23_P84344</t>
+  </si>
+  <si>
+    <t>A_23_P99275</t>
+  </si>
+  <si>
+    <t>A_24_P114739</t>
+  </si>
+  <si>
+    <t>A_24_P124831</t>
+  </si>
+  <si>
+    <t>A_24_P127462</t>
+  </si>
+  <si>
+    <t>A_24_P184031</t>
+  </si>
+  <si>
+    <t>A_24_P187583</t>
+  </si>
+  <si>
+    <t>A_24_P203000</t>
+  </si>
+  <si>
+    <t>A_24_P206848</t>
+  </si>
+  <si>
+    <t>A_24_P209455</t>
+  </si>
+  <si>
+    <t>A_24_P224926</t>
+  </si>
+  <si>
+    <t>A_24_P24819</t>
+  </si>
+  <si>
+    <t>A_24_P29975</t>
+  </si>
+  <si>
+    <t>A_24_P314451</t>
+  </si>
+  <si>
+    <t>A_24_P324563</t>
+  </si>
+  <si>
+    <t>A_24_P329353</t>
+  </si>
+  <si>
+    <t>A_24_P525917</t>
+  </si>
+  <si>
+    <t>A_24_P592871</t>
+  </si>
+  <si>
+    <t>A_24_P829107</t>
+  </si>
+  <si>
+    <t>A_24_P871726</t>
+  </si>
+  <si>
+    <t>A_24_P89457</t>
+  </si>
+  <si>
+    <t>A_24_P913146</t>
+  </si>
+  <si>
+    <t>A_24_P916288</t>
+  </si>
+  <si>
+    <t>A_24_P940348</t>
+  </si>
+  <si>
+    <t>A_24_P943393</t>
+  </si>
+  <si>
+    <t>A_32_P104746</t>
+  </si>
+  <si>
+    <t>A_32_P108554</t>
+  </si>
+  <si>
+    <t>A_32_P114284</t>
+  </si>
+  <si>
+    <t>A_32_P158966</t>
+  </si>
+  <si>
+    <t>A_32_P163247</t>
+  </si>
+  <si>
+    <t>A_32_P17343</t>
+  </si>
+  <si>
+    <t>A_32_P197060</t>
+  </si>
+  <si>
+    <t>A_32_P347617</t>
+  </si>
+  <si>
+    <t>A_32_P69492</t>
+  </si>
+  <si>
+    <t>A_32_P69956</t>
+  </si>
+  <si>
+    <t>A_32_P84009</t>
   </si>
 </sst>
 </file>
@@ -610,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1167,4 +1384,1143 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC5EF6C-1E83-4E9D-B5DC-DA9656558705}">
+  <dimension ref="A1:C140"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="1">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="1">
+        <v>621</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="1">
+        <v>699</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>1365</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>1487</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>1498</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>1692</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>1797</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>2094</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>2220</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>2231</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>2395</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>2444</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>2446</v>
+      </c>
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>2666</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>3147</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>3150</v>
+      </c>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>3168</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>3241</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
+        <v>3311</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
+        <v>3575</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>3785</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>3790</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>3984</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
+        <v>4062</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
+        <v>4185</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
+        <v>4203</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
+        <v>4557</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
+        <v>5188</v>
+      </c>
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="1">
+        <v>6444</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="1">
+        <v>6445</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="1">
+        <v>6571</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="1">
+        <v>6758</v>
+      </c>
+      <c r="C34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="1">
+        <v>6776</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="1">
+        <v>7034</v>
+      </c>
+      <c r="C36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="1">
+        <v>7113</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="1">
+        <v>7313</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="1">
+        <v>7505</v>
+      </c>
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="1">
+        <v>7637</v>
+      </c>
+      <c r="C40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="1">
+        <v>7678</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
+        <v>7709</v>
+      </c>
+      <c r="C42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="1">
+        <v>8213</v>
+      </c>
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="1">
+        <v>8224</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="1">
+        <v>8432</v>
+      </c>
+      <c r="C45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="1">
+        <v>8491</v>
+      </c>
+      <c r="C46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="1">
+        <v>8572</v>
+      </c>
+      <c r="C47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="1">
+        <v>8882</v>
+      </c>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="1">
+        <v>9091</v>
+      </c>
+      <c r="C49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="1">
+        <v>9314</v>
+      </c>
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="1">
+        <v>9354</v>
+      </c>
+      <c r="C51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="1">
+        <v>9394</v>
+      </c>
+      <c r="C52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="1">
+        <v>9498</v>
+      </c>
+      <c r="C53" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="1">
+        <v>9568</v>
+      </c>
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="1">
+        <v>10295</v>
+      </c>
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="1">
+        <v>10932</v>
+      </c>
+      <c r="C56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="1">
+        <v>11019</v>
+      </c>
+      <c r="C57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="1">
+        <v>11184</v>
+      </c>
+      <c r="C58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="1">
+        <v>11197</v>
+      </c>
+      <c r="C59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="1">
+        <v>11635</v>
+      </c>
+      <c r="C60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="1">
+        <v>12075</v>
+      </c>
+      <c r="C61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="1">
+        <v>12439</v>
+      </c>
+      <c r="C62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="1">
+        <v>12540</v>
+      </c>
+      <c r="C63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B64" s="1">
+        <v>12690</v>
+      </c>
+      <c r="C64" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="1">
+        <v>12965</v>
+      </c>
+      <c r="C65" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="1">
+        <v>12992</v>
+      </c>
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B67" s="1">
+        <v>13035</v>
+      </c>
+      <c r="C67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B68" s="1">
+        <v>13329</v>
+      </c>
+      <c r="C68" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B69" s="1">
+        <v>13955</v>
+      </c>
+      <c r="C69" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B70" s="1">
+        <v>14436</v>
+      </c>
+      <c r="C70" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B71" s="1">
+        <v>14526</v>
+      </c>
+      <c r="C71" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B72" s="1">
+        <v>14842</v>
+      </c>
+      <c r="C72" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B73" s="1">
+        <v>14850</v>
+      </c>
+      <c r="C73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B74" s="1">
+        <v>14922</v>
+      </c>
+      <c r="C74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B75" s="1">
+        <v>15004</v>
+      </c>
+      <c r="C75" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B76" s="1">
+        <v>15008</v>
+      </c>
+      <c r="C76" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B77" s="1">
+        <v>15038</v>
+      </c>
+      <c r="C77" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B78" s="1">
+        <v>15563</v>
+      </c>
+      <c r="C78" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="1">
+        <v>15818</v>
+      </c>
+      <c r="C79" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B80" s="1">
+        <v>15969</v>
+      </c>
+      <c r="C80" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" s="1">
+        <v>16053</v>
+      </c>
+      <c r="C81" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="1">
+        <v>16142</v>
+      </c>
+      <c r="C82" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B83" s="1">
+        <v>16264</v>
+      </c>
+      <c r="C83" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" s="1">
+        <v>16400</v>
+      </c>
+      <c r="C84" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B85" s="1">
+        <v>16404</v>
+      </c>
+      <c r="C85" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" s="1">
+        <v>16535</v>
+      </c>
+      <c r="C86" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B87" s="1">
+        <v>17044</v>
+      </c>
+      <c r="C87" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B88" s="1">
+        <v>17102</v>
+      </c>
+      <c r="C88" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B89" s="1">
+        <v>17201</v>
+      </c>
+      <c r="C89" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B90" s="1">
+        <v>17231</v>
+      </c>
+      <c r="C90" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B91" s="1">
+        <v>17420</v>
+      </c>
+      <c r="C91" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B92" s="1">
+        <v>17443</v>
+      </c>
+      <c r="C92" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B93" s="1">
+        <v>17502</v>
+      </c>
+      <c r="C93" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B94" s="1">
+        <v>18011</v>
+      </c>
+      <c r="C94" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B95" s="1">
+        <v>18235</v>
+      </c>
+      <c r="C95" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B96" s="1">
+        <v>18657</v>
+      </c>
+      <c r="C96" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B97" s="1">
+        <v>19084</v>
+      </c>
+      <c r="C97" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B98" s="1">
+        <v>19123</v>
+      </c>
+      <c r="C98" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B99" s="1">
+        <v>19372</v>
+      </c>
+      <c r="C99" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B100" s="1">
+        <v>19458</v>
+      </c>
+      <c r="C100" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B101" s="1">
+        <v>20803</v>
+      </c>
+      <c r="C101" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B102" s="1">
+        <v>20863</v>
+      </c>
+      <c r="C102" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B103" s="1">
+        <v>20967</v>
+      </c>
+      <c r="C103" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B104" s="1">
+        <v>21329</v>
+      </c>
+      <c r="C104" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B105" s="1">
+        <v>21468</v>
+      </c>
+      <c r="C105" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B106" s="1">
+        <v>21524</v>
+      </c>
+      <c r="C106" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B107" s="1">
+        <v>21904</v>
+      </c>
+      <c r="C107" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B108" s="1">
+        <v>21932</v>
+      </c>
+      <c r="C108" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B109" s="1">
+        <v>22415</v>
+      </c>
+      <c r="C109" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B110" s="1">
+        <v>22552</v>
+      </c>
+      <c r="C110" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B111" s="1">
+        <v>23795</v>
+      </c>
+      <c r="C111" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B112" s="1">
+        <v>24130</v>
+      </c>
+      <c r="C112" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B113" s="1">
+        <v>24429</v>
+      </c>
+      <c r="C113" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B114" s="1">
+        <v>24533</v>
+      </c>
+      <c r="C114" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B115" s="1">
+        <v>27031</v>
+      </c>
+      <c r="C115" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B116" s="1">
+        <v>27711</v>
+      </c>
+      <c r="C116" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B117" s="1">
+        <v>28267</v>
+      </c>
+      <c r="C117" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B118" s="1">
+        <v>30317</v>
+      </c>
+      <c r="C118" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B119" s="1">
+        <v>30704</v>
+      </c>
+      <c r="C119" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B120" s="1">
+        <v>30881</v>
+      </c>
+      <c r="C120" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B121" s="1">
+        <v>31161</v>
+      </c>
+      <c r="C121" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B122" s="1">
+        <v>31353</v>
+      </c>
+      <c r="C122" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B123" s="1">
+        <v>32053</v>
+      </c>
+      <c r="C123" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B124" s="1">
+        <v>32470</v>
+      </c>
+      <c r="C124" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B125" s="1">
+        <v>33030</v>
+      </c>
+      <c r="C125" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B126" s="1">
+        <v>33263</v>
+      </c>
+      <c r="C126" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B127" s="1">
+        <v>33431</v>
+      </c>
+      <c r="C127" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B128" s="1">
+        <v>33635</v>
+      </c>
+      <c r="C128" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B129" s="1">
+        <v>33764</v>
+      </c>
+      <c r="C129" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B130" s="1">
+        <v>33969</v>
+      </c>
+      <c r="C130" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B131" s="1">
+        <v>34440</v>
+      </c>
+      <c r="C131" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B132" s="1">
+        <v>35436</v>
+      </c>
+      <c r="C132" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B133" s="1">
+        <v>35581</v>
+      </c>
+      <c r="C133" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B134" s="1">
+        <v>35887</v>
+      </c>
+      <c r="C134" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B135" s="1">
+        <v>36591</v>
+      </c>
+      <c r="C135" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B136" s="1">
+        <v>38338</v>
+      </c>
+      <c r="C136" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B137" s="1">
+        <v>39805</v>
+      </c>
+      <c r="C137" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B138" s="1">
+        <v>39818</v>
+      </c>
+      <c r="C138" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B139" s="1">
+        <v>40376</v>
+      </c>
+      <c r="C139" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B140" s="1">
+        <v>40552</v>
+      </c>
+      <c r="C140" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>